<commit_message>
update matrix mult seq with one add one mult
</commit_message>
<xml_diff>
--- a/netlists/results/results.xlsx
+++ b/netlists/results/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Function</t>
   </si>
@@ -218,10 +218,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH23"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -661,33 +661,36 @@
         <v>1024</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="L10" s="6" t="n">
+      <c r="D10" s="6" t="n">
         <v>2047</v>
       </c>
-      <c r="M10" s="6" t="n">
+      <c r="E10" s="6" t="n">
         <v>2050</v>
       </c>
-      <c r="N10" s="6" t="n">
-        <f aca="false">L10+M10</f>
+      <c r="F10" s="6" t="n">
+        <f aca="false">SUM(D10:E10)</f>
         <v>4097</v>
       </c>
-      <c r="O10" s="6" t="n">
+      <c r="G10" s="6" t="n">
         <v>3070</v>
       </c>
-      <c r="P10" s="6" t="n">
-        <f aca="false">L10+M10+O10</f>
-        <v>7167</v>
-      </c>
-      <c r="Q10" s="5" t="n">
-        <f aca="false">N10+(O10*5)</f>
+      <c r="H10" s="6" t="n">
+        <f aca="false">SUM(D10:F10)</f>
+        <v>8194</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <f aca="false">(SUM(D10:E10)+5*G10)*I10</f>
         <v>19447</v>
       </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6" t="n">
         <f aca="false">U10-T10</f>
@@ -1033,6 +1036,7 @@
       <c r="V18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1078,6 +1082,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1123,6 +1128,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
       <c r="F21" s="6"/>
       <c r="H21" s="6"/>
       <c r="J21" s="5"/>
@@ -1131,6 +1138,8 @@
       <c r="V21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
       <c r="F22" s="6"/>
       <c r="H22" s="6"/>
       <c r="J22" s="5"/>
@@ -1143,35 +1152,96 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1026</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>1922</v>
+        <v>997</v>
       </c>
       <c r="F23" s="6" t="n">
         <f aca="false">SUM(D23:E23)</f>
-        <v>2948</v>
+        <v>2023</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>4050</v>
+        <v>1956</v>
       </c>
       <c r="H23" s="6" t="n">
         <f aca="false">SUM(D23:F23)</f>
-        <v>5896</v>
+        <v>4046</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>27</v>
+        <f aca="false">2*2*2</f>
+        <v>8</v>
       </c>
       <c r="J23" s="5" t="n">
         <f aca="false">(SUM(D23:E23)+5*G23)*I23</f>
-        <v>626346</v>
+        <v>94424</v>
       </c>
       <c r="N23" s="0"/>
       <c r="Q23" s="1"/>
       <c r="V23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1026</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>997</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <f aca="false">SUM(D24:E24)</f>
+        <v>2023</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1956</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <f aca="false">SUM(D24:F24)</f>
+        <v>4046</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">3*3*3</f>
+        <v>27</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <f aca="false">(SUM(D24:E24)+5*G24)*I24</f>
+        <v>318681</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1026</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>997</v>
+      </c>
+      <c r="F25" s="6" t="n">
+        <f aca="false">SUM(D25:E25)</f>
+        <v>2023</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>1956</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">SUM(D25:F25)</f>
+        <v>4046</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <f aca="false">5*5*5</f>
+        <v>125</v>
+      </c>
+      <c r="J25" s="5" t="n">
+        <f aca="false">(SUM(D25:E25)+5*G25)*I25</f>
+        <v>1475375</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>